<commit_message>
top 10 wordcounts in RDD
</commit_message>
<xml_diff>
--- a/visual_results.xlsx
+++ b/visual_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S537159\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\semester4_files\BigData\spark-installation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,31 +26,31 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>dementor</t>
+    <t xml:space="preserve">have </t>
   </si>
   <si>
-    <t>filled</t>
+    <t>the</t>
   </si>
   <si>
-    <t>we</t>
+    <t>of</t>
   </si>
   <si>
-    <t>light</t>
+    <t>a</t>
   </si>
   <si>
-    <t>Newman</t>
+    <t>and</t>
   </si>
   <si>
-    <t>out</t>
+    <t>The</t>
   </si>
   <si>
-    <t>cold</t>
+    <t>was</t>
   </si>
   <si>
-    <t>as</t>
+    <t>to</t>
   </si>
   <si>
-    <t xml:space="preserve">have </t>
+    <t>at</t>
   </si>
 </sst>
 </file>
@@ -216,28 +216,28 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>dementor</c:v>
+                  <c:v>the</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>filled</c:v>
+                  <c:v>of</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>we</c:v>
+                  <c:v>a</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>light</c:v>
+                  <c:v>and</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Newman</c:v>
+                  <c:v>The</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>out</c:v>
+                  <c:v>was</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>cold</c:v>
+                  <c:v>to</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>as</c:v>
+                  <c:v>at</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>have </c:v>
@@ -252,28 +252,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>9</c:v>
@@ -1296,7 +1296,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,71 +1306,71 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B9">
         <v>9</v>

</xml_diff>